<commit_message>
Final version for 1 student per slot
</commit_message>
<xml_diff>
--- a/DataFiles/ProcessingWorkbook_1.xlsx
+++ b/DataFiles/ProcessingWorkbook_1.xlsx
@@ -1277,22 +1277,22 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>Providence Health Network</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
           <t>Cedars-Sinai - Neurosciences</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>Keck VIO - COBI</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>Optum CF - Patient XP</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Providence Health Network</t>
         </is>
       </c>
     </row>
@@ -1342,17 +1342,17 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
+          <t>Rancho Los Amigos NRC</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
           <t>CHLA - Anesthesia&amp;CCM</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>Providence Health Network</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Optum CF - Patient XP</t>
         </is>
       </c>
     </row>
@@ -1372,12 +1372,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
+          <t>Emanate Health</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
           <t>Cedars-Sinai - Neurosciences</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Emanate Health</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -1407,12 +1407,12 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
+          <t>Verdugo Hills Hospital</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
           <t>Keck VIO - COBI</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Kaiser PC - Consulting</t>
         </is>
       </c>
     </row>
@@ -1437,7 +1437,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>SCAN Health Plan</t>
+          <t>Providence Health Network</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -1462,17 +1462,17 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
+          <t>CHLA - Anesthesia&amp;CCM</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
           <t>City of Hope - CMO</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>CHLA - Anesthesia&amp;CCM</t>
-        </is>
-      </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t xml:space="preserve">St.Johns-PhysPartners </t>
+          <t>Rancho Los Amigos NRC</t>
         </is>
       </c>
     </row>
@@ -1487,22 +1487,22 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Providence Health Network</t>
+          <t>Cedars-Sinai - Neurosciences</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>SCAN Health Plan</t>
+          <t>Keck VIO - COBI</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Cedars-Sinai - Neurosciences</t>
+          <t>Optum CF - Patient XP</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Keck VIO - COBI</t>
+          <t xml:space="preserve">St.Johns-PhysPartners </t>
         </is>
       </c>
     </row>
@@ -1592,7 +1592,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Rancho Los Amigos NRC</t>
+          <t>Torrance Memorial</t>
         </is>
       </c>
     </row>
@@ -1690,17 +1690,17 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>Raashi Subramanya</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
           <t>Oceana Hanner</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>Fahima Gohil</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Raashi Subramanya</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -1723,12 +1723,12 @@
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
+          <t>Stanley Ibe</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
           <t>Daniela Ahumada</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Stanley Ibe</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -1753,12 +1753,12 @@
           <t>Daniela Ahumada</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
         <is>
           <t>Stanley Ibe</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
           <t>Fahima Gohil</t>
@@ -1781,12 +1781,12 @@
           <t>Julia Orozco</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>Fahima Gohil</t>
         </is>
       </c>
+      <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
     </row>
     <row r="6">
@@ -1815,11 +1815,7 @@
           <t>Nikhil Bajpai</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Julia Orozco</t>
-        </is>
-      </c>
+      <c r="F6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1863,17 +1859,17 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
+          <t>Raashi Subramanya</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
           <t>Oceana Hanner</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>Julia Orozco</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>Raashi Subramanya</t>
         </is>
       </c>
     </row>
@@ -1924,12 +1920,12 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
+          <t>Raashi Subramanya</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
           <t>Oceana Hanner</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>Daniela Ahumada</t>
         </is>
       </c>
     </row>
@@ -1946,7 +1942,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Raashi Subramanya</t>
+          <t>Oceana Hanner</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1956,12 +1952,12 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
+          <t>Emma Crusinberry</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
           <t>Daniela Ahumada</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>Oceana Hanner</t>
         </is>
       </c>
     </row>
@@ -1981,7 +1977,11 @@
           <t>Fahima Gohil</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr"/>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Daniela Ahumada</t>
+        </is>
+      </c>
       <c r="E12" t="inlineStr">
         <is>
           <t xml:space="preserve"> Bryce Dechert</t>
@@ -1989,7 +1989,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Russelle Chang</t>
+          <t>Stanley Ibe</t>
         </is>
       </c>
     </row>
@@ -2005,16 +2005,8 @@
         </is>
       </c>
       <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>Raashi Subramanya</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>Emma Crusinberry</t>
-        </is>
-      </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
     </row>
     <row r="14">
@@ -2041,7 +2033,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Stanley Ibe</t>
+          <t>Raashi Subramanya</t>
         </is>
       </c>
     </row>
@@ -2063,7 +2055,11 @@
       </c>
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr"/>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Russelle Chang</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2086,7 +2082,11 @@
           <t xml:space="preserve"> Bryce Dechert</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr"/>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Julia Orozco</t>
+        </is>
+      </c>
       <c r="F16" t="inlineStr">
         <is>
           <t>Nikhil Bajpai</t>

</xml_diff>

<commit_message>
Multi slots per student handling
</commit_message>
<xml_diff>
--- a/DataFiles/ProcessingWorkbook_1.xlsx
+++ b/DataFiles/ProcessingWorkbook_1.xlsx
@@ -1277,17 +1277,17 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>Keck VIO - COBI</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Cedars-Sinai - Neurosciences</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
           <t>Providence Health Network</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Cedars-Sinai - Neurosciences</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Keck VIO - COBI</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -1307,22 +1307,22 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t xml:space="preserve">St.Johns-PhysPartners </t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Optum CF - Patient XP</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Verdugo Hills Hospital</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
           <t>Keck VIO - COBI</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Optum CF - Patient XP</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">St.Johns-PhysPartners </t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>West Hills Hospital</t>
         </is>
       </c>
     </row>
@@ -1337,22 +1337,22 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
+          <t>CHLA - Anesthesia&amp;CCM</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
           <t>City of Hope - CMO</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>Rancho Los Amigos NRC</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>CHLA - Anesthesia&amp;CCM</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Providence Health Network</t>
         </is>
       </c>
     </row>
@@ -1367,22 +1367,22 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
+          <t>City of Hope - CMO</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Emanate Health</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Cedars-Sinai - Neurosciences</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
           <t>Rancho Los Amigos NRC</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Emanate Health</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Cedars-Sinai - Neurosciences</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>City of Hope - CMO</t>
         </is>
       </c>
     </row>
@@ -1407,12 +1407,12 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Verdugo Hills Hospital</t>
+          <t>Keck VIO - COBI</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Keck VIO - COBI</t>
+          <t>Kaiser PC - Consulting</t>
         </is>
       </c>
     </row>
@@ -1437,7 +1437,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Providence Health Network</t>
+          <t>SCAN Health Plan</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -1472,7 +1472,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Rancho Los Amigos NRC</t>
+          <t xml:space="preserve">St.Johns-PhysPartners </t>
         </is>
       </c>
     </row>
@@ -1502,7 +1502,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t xml:space="preserve">St.Johns-PhysPartners </t>
+          <t>Providence Health Network</t>
         </is>
       </c>
     </row>
@@ -1592,7 +1592,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Torrance Memorial</t>
+          <t>City of Hope - CMO</t>
         </is>
       </c>
     </row>
@@ -1617,12 +1617,12 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Rancho Los Amigos NRC</t>
+          <t>CHLA - Anesthesia&amp;CCM</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>CHLA - Anesthesia&amp;CCM</t>
+          <t>Optum CF - Digi Transformation</t>
         </is>
       </c>
     </row>
@@ -1637,7 +1637,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1720,7 +1720,11 @@
           <t>CHLA - Anesthesia&amp;CCM</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr"/>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Daniela Ahumada</t>
+        </is>
+      </c>
       <c r="D3" t="inlineStr">
         <is>
           <t>Stanley Ibe</t>
@@ -1728,12 +1732,12 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Bryce Dechert</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
           <t>Daniela Ahumada</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Bryce Dechert</t>
         </is>
       </c>
     </row>
@@ -1750,10 +1754,14 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
+          <t>Fahima Gohil</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
           <t>Daniela Ahumada</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr">
         <is>
           <t>Stanley Ibe</t>
@@ -1761,7 +1769,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Fahima Gohil</t>
+          <t>Russelle Chang</t>
         </is>
       </c>
     </row>
@@ -1815,7 +1823,11 @@
           <t>Nikhil Bajpai</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr"/>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Julia Orozco</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1840,6 +1852,7 @@
           <t>Eryn Burnette</t>
         </is>
       </c>
+      <c r="G7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1854,22 +1867,22 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
+          <t>Oceana Hanner</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Raashi Subramanya</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Julia Orozco</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
           <t>Esther Choi</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Raashi Subramanya</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Oceana Hanner</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>Julia Orozco</t>
         </is>
       </c>
     </row>
@@ -1895,7 +1908,11 @@
           <t>Russelle Chang</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr"/>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Bryce Dechert</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1940,24 +1957,20 @@
           <t>Providence Health Network</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Julia Orozco</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
         <is>
           <t>Oceana Hanner</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Julia Orozco</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Emma Crusinberry</t>
-        </is>
-      </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Daniela Ahumada</t>
+          <t>Raashi Subramanya</t>
         </is>
       </c>
     </row>
@@ -1972,24 +1985,16 @@
           <t>Rancho Los Amigos NRC</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Daniela Ahumada</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
         <is>
           <t>Fahima Gohil</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>Daniela Ahumada</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Bryce Dechert</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>Stanley Ibe</t>
         </is>
       </c>
     </row>
@@ -2006,7 +2011,11 @@
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Emma Crusinberry</t>
+        </is>
+      </c>
       <c r="F13" t="inlineStr"/>
     </row>
     <row r="14">
@@ -2020,20 +2029,20 @@
           <t xml:space="preserve">St.Johns-PhysPartners </t>
         </is>
       </c>
-      <c r="C14" t="inlineStr"/>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Esther Choi</t>
+        </is>
+      </c>
       <c r="D14" t="inlineStr">
         <is>
           <t>Emma Crusinberry</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>Esther Choi</t>
-        </is>
-      </c>
+      <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Raashi Subramanya</t>
+          <t>Stanley Ibe</t>
         </is>
       </c>
     </row>
@@ -2055,11 +2064,7 @@
       </c>
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>Russelle Chang</t>
-        </is>
-      </c>
+      <c r="F15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2084,7 +2089,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Julia Orozco</t>
+          <t>Esther Choi</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -2119,11 +2124,7 @@
           <t>Eryn Burnette</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>Esther Choi</t>
-        </is>
-      </c>
+      <c r="F17" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>